<commit_message>
import updated but still not working, error message
</commit_message>
<xml_diff>
--- a/public/DataArsip/(Template) Arsip Tekstual web.xlsx
+++ b/public/DataArsip/(Template) Arsip Tekstual web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Users\bar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900AB09D-8CBB-4FF2-9CF1-8F192DC92090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F215051A-844C-4608-92D6-9A0708678AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,34 +205,34 @@
     <t>KODE PELAKSANA</t>
   </si>
   <si>
+    <t>TINGKAT PERKEMBANGAN</t>
+  </si>
+  <si>
+    <t>MEDIA SIMPAN</t>
+  </si>
+  <si>
+    <t>JUMLAH BERKAS</t>
+  </si>
+  <si>
+    <t>KONDISI FISIK</t>
+  </si>
+  <si>
+    <t>Ukuran</t>
+  </si>
+  <si>
+    <t>Ruang</t>
+  </si>
+  <si>
+    <t>Lemari</t>
+  </si>
+  <si>
+    <t>Boks</t>
+  </si>
+  <si>
+    <t>Jenis Arsip</t>
+  </si>
+  <si>
     <t>Nomor Arsip</t>
-  </si>
-  <si>
-    <t>TINGKAT PERKEMBANGAN</t>
-  </si>
-  <si>
-    <t>MEDIA SIMPAN</t>
-  </si>
-  <si>
-    <t>JUMLAH BERKAS</t>
-  </si>
-  <si>
-    <t>KONDISI FISIK</t>
-  </si>
-  <si>
-    <t>Ukuran</t>
-  </si>
-  <si>
-    <t>Ruang</t>
-  </si>
-  <si>
-    <t>Lemari</t>
-  </si>
-  <si>
-    <t>Boks</t>
-  </si>
-  <si>
-    <t>Jenis Arsip</t>
   </si>
 </sst>
 </file>
@@ -665,8 +665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="A3:F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,7 +695,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="34.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>58</v>
@@ -718,34 +719,34 @@
         <v>3</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>6</v>
@@ -1989,10 +1990,10 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Data!$B$2:$B$19</xm:f>

</xml_diff>